<commit_message>
Records with wrong dates were corrected.
There was 1 date with 1930 as the year and 2 other dates with 1930 as their year. The year in all three dates was changed to 2021 as 2021 is the only year that is covered in this dataset.
</commit_message>
<xml_diff>
--- a/Normalization of Sales Data Table/block_sales_2021.xlsx
+++ b/Normalization of Sales Data Table/block_sales_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\My_Works\My_Github_Repos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\My_Works\My_Github_Repos\Ridhwan_Repo\Normalization of Sales Data Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FB3FB2-576D-4C87-A8AC-888F805CFD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F912B7FF-486D-4D13-9923-8D725CBB3A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6100,7 +6100,7 @@
         <v>20210157</v>
       </c>
       <c r="B158" s="1">
-        <v>11036</v>
+        <v>44274</v>
       </c>
       <c r="C158" t="s">
         <v>2</v>
@@ -13723,7 +13723,7 @@
         <v>2</v>
       </c>
       <c r="D389">
-        <f t="shared" ref="D387:D450" si="6">IF(C389 = "4 inches",200,IF(C389="6 inches",250,IF(C389="9 inches",300)))</f>
+        <f t="shared" ref="D389:D450" si="6">IF(C389 = "4 inches",200,IF(C389="6 inches",250,IF(C389="9 inches",300)))</f>
         <v>200</v>
       </c>
       <c r="E389">
@@ -14674,7 +14674,7 @@
         <v>20210417</v>
       </c>
       <c r="B418" s="1">
-        <v>11173</v>
+        <v>44410</v>
       </c>
       <c r="C418" t="s">
         <v>0</v>
@@ -18831,7 +18831,7 @@
         <v>20210543</v>
       </c>
       <c r="B544" s="1">
-        <v>4</v>
+        <v>44473</v>
       </c>
       <c r="C544" t="s">
         <v>1</v>

</xml_diff>